<commit_message>
Done find Book; update Staff
</commit_message>
<xml_diff>
--- a/src/main/java/com/example/librarymanagement/LibraryManagement.xlsx
+++ b/src/main/java/com/example/librarymanagement/LibraryManagement.xlsx
@@ -26,9 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="84">
   <si>
-    <t>Tìm kiếm theo tên || Tìm kiếm theo nhà xuất bản || Tìm kiếm theo tác giả: Books</t>
-  </si>
-  <si>
     <t>Tìm kiếm theo mã độc giả || Tìm kiếm theo tên độc giả: độc giả</t>
   </si>
   <si>
@@ -336,6 +333,9 @@
   </si>
   <si>
     <t>Hiển thị danh sách sách trong phiếu mượn: void</t>
+  </si>
+  <si>
+    <t>Tìm kiếm theo mã sách || Tìm kiếm theo tên || Tìm kiếm theo nhà xuất bản || Tìm kiếm theo tác giả: Books</t>
   </si>
 </sst>
 </file>
@@ -817,7 +817,7 @@
   <dimension ref="A1:R48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="A19" sqref="A19:A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -839,27 +839,27 @@
     <row r="1" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F2" s="9"/>
       <c r="G2" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H2" s="9"/>
       <c r="I2" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J2" s="9"/>
       <c r="K2" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L2" s="7"/>
       <c r="M2" s="7"/>
@@ -871,27 +871,27 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H3" s="7"/>
       <c r="I3" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J3" s="7"/>
       <c r="K3" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L3" s="7"/>
       <c r="M3" s="7"/>
@@ -903,27 +903,27 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H4" s="7"/>
       <c r="I4" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J4" s="7"/>
       <c r="K4" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
@@ -935,27 +935,27 @@
     </row>
     <row r="5" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H5" s="7"/>
       <c r="I5" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J5" s="7"/>
       <c r="K5" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
@@ -967,27 +967,27 @@
     </row>
     <row r="6" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J6" s="7"/>
       <c r="K6" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
@@ -999,27 +999,27 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H7" s="7"/>
       <c r="I7" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J7" s="7"/>
       <c r="K7" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L7" s="7"/>
       <c r="M7" s="7"/>
@@ -1031,27 +1031,27 @@
     </row>
     <row r="8" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H8" s="7"/>
       <c r="I8" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J8" s="7"/>
       <c r="K8" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L8" s="7"/>
       <c r="M8" s="7"/>
@@ -1063,25 +1063,25 @@
     </row>
     <row r="9" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
       <c r="G9" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H9" s="7"/>
       <c r="I9" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J9" s="7"/>
       <c r="K9" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L9" s="7"/>
       <c r="M9" s="7"/>
@@ -1093,7 +1093,7 @@
     </row>
     <row r="10" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -1103,11 +1103,11 @@
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
       <c r="I10" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J10" s="7"/>
       <c r="K10" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L10" s="7"/>
       <c r="M10" s="7"/>
@@ -1119,7 +1119,7 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -1129,11 +1129,11 @@
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
       <c r="I11" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J11" s="7"/>
       <c r="K11" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L11" s="7"/>
       <c r="M11" s="7"/>
@@ -1145,7 +1145,7 @@
     </row>
     <row r="12" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -1155,11 +1155,11 @@
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
       <c r="I12" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J12" s="7"/>
       <c r="K12" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L12" s="7"/>
       <c r="M12" s="7"/>
@@ -1171,7 +1171,7 @@
     </row>
     <row r="13" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
@@ -1183,7 +1183,7 @@
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
       <c r="K13" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L13" s="7"/>
       <c r="M13" s="7"/>
@@ -1255,27 +1255,27 @@
     </row>
     <row r="17" spans="1:18" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B17" s="9"/>
       <c r="C17" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D17" s="9"/>
       <c r="E17" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F17" s="9"/>
       <c r="G17" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H17" s="9"/>
       <c r="I17" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J17" s="9"/>
       <c r="K17" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L17" s="7"/>
       <c r="M17" s="7"/>
@@ -1287,27 +1287,27 @@
     </row>
     <row r="18" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B18" s="7"/>
       <c r="C18" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H18" s="7"/>
       <c r="I18" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J18" s="7"/>
       <c r="K18" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L18" s="7"/>
       <c r="M18" s="7"/>
@@ -1319,25 +1319,25 @@
     </row>
     <row r="19" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="19" t="s">
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="B19" s="7"/>
       <c r="C19" s="22" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
       <c r="I19" s="19" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J19" s="7"/>
       <c r="K19" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L19" s="7"/>
       <c r="M19" s="7"/>
@@ -1353,7 +1353,7 @@
       <c r="C20" s="23"/>
       <c r="D20" s="7"/>
       <c r="E20" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
@@ -1361,7 +1361,7 @@
       <c r="I20" s="20"/>
       <c r="J20" s="7"/>
       <c r="K20" s="19" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L20" s="7"/>
       <c r="M20" s="7"/>
@@ -1377,7 +1377,7 @@
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
       <c r="E21" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
@@ -1425,7 +1425,7 @@
       <c r="I23" s="7"/>
       <c r="J23" s="7"/>
       <c r="K23" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L23" s="7"/>
       <c r="M23" s="7"/>
@@ -1477,7 +1477,7 @@
     </row>
     <row r="26" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
@@ -1499,7 +1499,7 @@
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
@@ -1521,7 +1521,7 @@
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
@@ -1543,7 +1543,7 @@
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
@@ -1565,7 +1565,7 @@
     </row>
     <row r="30" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
@@ -1615,11 +1615,11 @@
       <c r="G32" s="7"/>
       <c r="H32" s="7"/>
       <c r="I32" s="14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J32" s="7"/>
       <c r="K32" s="14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L32" s="7"/>
       <c r="M32" s="7"/>
@@ -1659,11 +1659,11 @@
       <c r="G34" s="7"/>
       <c r="H34" s="7"/>
       <c r="I34" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J34" s="7"/>
       <c r="K34" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L34" s="7"/>
       <c r="M34" s="7"/>
@@ -1682,11 +1682,11 @@
       <c r="G35" s="7"/>
       <c r="H35" s="7"/>
       <c r="I35" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J35" s="7"/>
       <c r="K35" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L35" s="7"/>
       <c r="M35" s="7"/>
@@ -1743,10 +1743,10 @@
     </row>
     <row r="39" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I39" s="18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K39" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="40" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1755,27 +1755,27 @@
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.3">
       <c r="I41" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I42" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K42" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="45" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I45" s="18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K45" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="46" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1784,18 +1784,18 @@
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.3">
       <c r="I47" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="48" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I48" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K48" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Done login and menu
</commit_message>
<xml_diff>
--- a/src/main/java/com/example/librarymanagement/LibraryManagement.xlsx
+++ b/src/main/java/com/example/librarymanagement/LibraryManagement.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="85">
   <si>
     <t>Tìm kiếm theo mã độc giả || Tìm kiếm theo tên độc giả: độc giả</t>
   </si>
@@ -249,9 +249,6 @@
   </si>
   <si>
     <t>edit(T t, T t): void</t>
-  </si>
-  <si>
-    <t>show(): void</t>
   </si>
   <si>
     <t>IManagement &lt;T t&gt;</t>
@@ -336,6 +333,12 @@
   </si>
   <si>
     <t>Tìm kiếm theo mã sách || Tìm kiếm theo tên || Tìm kiếm theo nhà xuất bản || Tìm kiếm theo tác giả: Books</t>
+  </si>
+  <si>
+    <t>Tự động chuyển đổi trạng thái khi quá hạn(String id, Reader reader)</t>
+  </si>
+  <si>
+    <t>findIndexById: void</t>
   </si>
 </sst>
 </file>
@@ -816,8 +819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:A21"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1255,11 +1258,11 @@
     </row>
     <row r="17" spans="1:18" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B17" s="9"/>
       <c r="C17" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D17" s="9"/>
       <c r="E17" s="10" t="s">
@@ -1267,15 +1270,15 @@
       </c>
       <c r="F17" s="9"/>
       <c r="G17" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="H17" s="9"/>
+      <c r="I17" s="14" t="s">
         <v>79</v>
-      </c>
-      <c r="H17" s="9"/>
-      <c r="I17" s="10" t="s">
-        <v>80</v>
       </c>
       <c r="J17" s="9"/>
       <c r="K17" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L17" s="7"/>
       <c r="M17" s="7"/>
@@ -1319,7 +1322,7 @@
     </row>
     <row r="19" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B19" s="7"/>
       <c r="C19" s="22" t="s">
@@ -1333,7 +1336,7 @@
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
       <c r="I19" s="19" t="s">
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="J19" s="7"/>
       <c r="K19" s="11" t="s">
@@ -1377,12 +1380,12 @@
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
       <c r="E21" s="20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
-      <c r="I21" s="21"/>
+      <c r="I21" s="2"/>
       <c r="J21" s="7"/>
       <c r="K21" s="20"/>
       <c r="L21" s="7"/>
@@ -1402,7 +1405,9 @@
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
+      <c r="I22" s="20" t="s">
+        <v>0</v>
+      </c>
       <c r="J22" s="7"/>
       <c r="K22" s="20"/>
       <c r="L22" s="7"/>
@@ -1422,7 +1427,7 @@
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
+      <c r="I23" s="20"/>
       <c r="J23" s="7"/>
       <c r="K23" s="3" t="s">
         <v>5</v>
@@ -1435,7 +1440,7 @@
       <c r="Q23" s="7"/>
       <c r="R23" s="7"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
@@ -1444,7 +1449,7 @@
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
+      <c r="I24" s="21"/>
       <c r="J24" s="7"/>
       <c r="K24" s="7"/>
       <c r="L24" s="7"/>
@@ -1477,7 +1482,7 @@
     </row>
     <row r="26" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
@@ -1565,7 +1570,7 @@
     </row>
     <row r="30" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="17" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
@@ -1799,12 +1804,13 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="A19:A21"/>
     <mergeCell ref="K20:K22"/>
-    <mergeCell ref="I19:I21"/>
+    <mergeCell ref="I22:I24"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="E21:E22"/>
+    <mergeCell ref="I19:I20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>